<commit_message>
added classes for tkinter, cleaned up main.py
</commit_message>
<xml_diff>
--- a/Exports/s24_mechelv.xlsx
+++ b/Exports/s24_mechelv.xlsx
@@ -108,8 +108,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="5213751185669702476" xfId="1" hidden="0"/>
-    <cellStyle name="-1363475798069386395" xfId="2" hidden="0"/>
+    <cellStyle name="362528962533712342" xfId="1" hidden="0"/>
+    <cellStyle name="4337898275422831775" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>

<commit_message>
add more excel exports, add tk_interface.py
</commit_message>
<xml_diff>
--- a/Exports/s24_mechelv.xlsx
+++ b/Exports/s24_mechelv.xlsx
@@ -108,8 +108,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="362528962533712342" xfId="1" hidden="0"/>
-    <cellStyle name="4337898275422831775" xfId="2" hidden="0"/>
+    <cellStyle name="4565284716643894420" xfId="1" hidden="0"/>
+    <cellStyle name="-5412700539081648563" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>